<commit_message>
Retrieve Metadata - using "mdapi" topic
</commit_message>
<xml_diff>
--- a/me/1.SFDX-Project.xlsx
+++ b/me/1.SFDX-Project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\SFDX-and-Salesforce-CLI\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51604E8B-FD22-4908-AB21-B8B6F49A9374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6101B28-F08A-46D3-ACD2-E691EE3721C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create SFDX Project" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="110">
   <si>
     <t>sfdx force:project:create --help</t>
   </si>
@@ -224,9 +224,6 @@
   </si>
   <si>
     <t>        &lt;name&gt;CustomTab&lt;/name&gt;</t>
-  </si>
-  <si>
-    <t>    &lt;version&gt;55.0&lt;/version&gt;</t>
   </si>
   <si>
     <t>&lt;/Package&gt;</t>
@@ -593,6 +590,24 @@
       <t>=sfdx</t>
     </r>
   </si>
+  <si>
+    <t>構成</t>
+  </si>
+  <si>
+    <t>CLISession</t>
+  </si>
+  <si>
+    <t>.sfdx</t>
+  </si>
+  <si>
+    <t>sfdx-config.json</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>    &lt;version&gt;46.0&lt;/version&gt;</t>
+  </si>
 </sst>
 </file>
 
@@ -614,12 +629,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -714,7 +735,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -731,6 +752,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -997,13 +1021,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>152401</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>38101</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>419101</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>116729</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1041,13 +1065,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>265462</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>95106</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1085,13 +1109,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1138,13 +1162,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1191,13 +1215,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1244,13 +1268,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>70</xdr:row>
+      <xdr:row>80</xdr:row>
       <xdr:rowOff>93664</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1288,13 +1312,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1341,13 +1365,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>72</xdr:row>
+      <xdr:row>82</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>427439</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:row>89</xdr:row>
       <xdr:rowOff>133175</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1385,13 +1409,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>92</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1438,13 +1462,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1491,13 +1515,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>85</xdr:row>
+      <xdr:row>95</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1544,13 +1568,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1861,8 +1885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A4:T198"/>
   <sheetViews>
-    <sheetView topLeftCell="A175" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O188" sqref="O188"/>
+    <sheetView tabSelected="1" topLeftCell="A169" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B174" sqref="B174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2571,13 +2595,13 @@
     </row>
     <row r="173" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B173" s="4" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="I173" s="5"/>
     </row>
     <row r="174" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B174" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C174" s="8"/>
       <c r="D174" s="8"/>
@@ -2589,10 +2613,10 @@
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I177" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.25">
@@ -2607,67 +2631,67 @@
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B179" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G179" s="5"/>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B180" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G180" s="5"/>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B181" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G181" s="5"/>
       <c r="H181" t="s">
         <v>19</v>
       </c>
       <c r="I181" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B182" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G182" s="5"/>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B183" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G183" s="5"/>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B184" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G184" s="5"/>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B185" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G185" s="5"/>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B186" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G186" s="5"/>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B187" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G187" s="5"/>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B188" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G188" s="5"/>
     </row>
@@ -2679,7 +2703,7 @@
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B190" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G190" s="5"/>
     </row>
@@ -2695,22 +2719,22 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2722,37 +2746,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D56C9DB-4648-44EE-BBB4-80763579E511}">
-  <dimension ref="A2:M87"/>
+  <dimension ref="A2:M97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S73" sqref="S73"/>
+    <sheetView topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -2760,13 +2784,13 @@
       <c r="L5" s="2"/>
       <c r="M5" s="3"/>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
@@ -2778,13 +2802,13 @@
       <c r="L6" s="8"/>
       <c r="M6" s="9"/>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
@@ -2796,113 +2820,255 @@
       <c r="L7" s="8"/>
       <c r="M7" s="9"/>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="16"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="C12" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" s="16"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="10"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" s="14" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="14" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B55" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="3"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B56" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F56" s="5"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B57" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C57" s="8"/>
+      <c r="D57" s="8"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="9"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="3"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B46" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C46" s="15"/>
-      <c r="D46" s="15"/>
-      <c r="E46" s="15"/>
-      <c r="F46" s="5"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B47" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
-      <c r="F47" s="9"/>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B72" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B94" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C94" s="2"/>
+      <c r="D94" s="2"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="3"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B95" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B84" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C84" s="2"/>
-      <c r="D84" s="2"/>
-      <c r="E84" s="2"/>
-      <c r="F84" s="3"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B85" s="4" t="s">
+      <c r="F95" s="5"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B96" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="C85" s="15"/>
-      <c r="D85" s="15"/>
-      <c r="E85" s="15"/>
-      <c r="F85" s="5"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B86" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="C86" s="15"/>
-      <c r="D86" s="15"/>
-      <c r="E86" s="15"/>
-      <c r="F86" s="5"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B87" s="10" t="s">
+      <c r="F96" s="5"/>
+    </row>
+    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B97" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C87" s="8"/>
-      <c r="D87" s="8"/>
-      <c r="E87" s="8"/>
-      <c r="F87" s="9"/>
+      <c r="C97" s="8"/>
+      <c r="D97" s="8"/>
+      <c r="E97" s="8"/>
+      <c r="F97" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>